<commit_message>
Atualização casos de teste e adição burn
</commit_message>
<xml_diff>
--- a/documentacao/TabelaTestes/TabeladeTestes_Sprint3.xlsx
+++ b/documentacao/TabelaTestes/TabeladeTestes_Sprint3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\Documents\SENAI\JavaScript\PROJETOS\TCC\documentacao\TabelaTestes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1171A66-CFFA-43C7-B5F5-8A9BD9CAD610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D16FF7F-E323-4F59-83F6-876F0F8C7C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Caso de Teste 1</t>
   </si>
@@ -76,6 +76,42 @@
   </si>
   <si>
     <t>Funcionalidade:  Realizar a visualização dos hospitais cadastrados no mapa.</t>
+  </si>
+  <si>
+    <t>Caso de Teste 2</t>
+  </si>
+  <si>
+    <t>Preencher o campo "descrição"</t>
+  </si>
+  <si>
+    <t>Funcionalidade:  Possibilitar ao paciente uma forma de fazer a solicitação de atendimento aos hospitais próximos.</t>
+  </si>
+  <si>
+    <t>Apertar no botão de solicitação (se encontra ao lado do campo "descrição")</t>
+  </si>
+  <si>
+    <t>Visualizar confirmação do APP, afirmando que a solicitação foi enviada com sucesso</t>
+  </si>
+  <si>
+    <t>Possibilitar ao paciente que envie a devida solicitação de atendimento aos hospitais</t>
+  </si>
+  <si>
+    <t>Caso de Teste 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcionalidade: Permitir que hospitais que receberam a solicitação, tenham acesso aos dados do paciente (nome, bio, cpf, etc.). </t>
+  </si>
+  <si>
+    <t>Acessar página de gerenciamento do hospital</t>
+  </si>
+  <si>
+    <t>Verificar a solicitação do paciente, juntamente com os devidos dados dele ( nome, bio, cpf, etc.)</t>
+  </si>
+  <si>
+    <t>Fracasso</t>
+  </si>
+  <si>
+    <t>Permitir que os hospitais visualizem a solicitação, juntamente com os  respectivos dados do paciente</t>
   </si>
 </sst>
 </file>
@@ -119,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -168,11 +204,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,10 +236,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -202,6 +255,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -489,28 +545,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D9:F19"/>
+  <dimension ref="D9:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="6" max="6" width="68.140625" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1"/>
     <col min="12" max="12" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D10" s="7" t="s">
@@ -523,60 +580,60 @@
       <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D13" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D14" s="4">
         <v>3</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
@@ -600,8 +657,216 @@
         <v>6</v>
       </c>
     </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="6">
+        <v>2</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="6">
+        <v>3</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="6">
+        <v>4</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="6">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3">
+        <v>43980</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="6">
+        <v>1</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="6">
+        <v>2</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="6">
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <v>43980</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="27">
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="E16:F16"/>
@@ -613,5 +878,6 @@
     <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>